<commit_message>
Add slide 2 item prices into excel sheet
</commit_message>
<xml_diff>
--- a/menu_data.xlsx
+++ b/menu_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin\Documents\Lirui_Menu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ACD3CCE4-64AC-468C-8F77-90080A113B4E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73913F39-C838-404C-93DA-93BCDE0A3601}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8880" yWindow="3495" windowWidth="28800" windowHeight="15435" xr2:uid="{D1279C1E-2E76-4EC6-A8DD-75E7E856264E}"/>
+    <workbookView xWindow="7215" yWindow="3600" windowWidth="28800" windowHeight="15435" xr2:uid="{D1279C1E-2E76-4EC6-A8DD-75E7E856264E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,6 +27,44 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Chicken</t>
+  </si>
+  <si>
+    <t>Shrimp</t>
+  </si>
+  <si>
+    <t>Beef &amp; shrimp</t>
+  </si>
+  <si>
+    <t>Beef</t>
+  </si>
+  <si>
+    <t>Chicken &amp; Shrimp</t>
+  </si>
+  <si>
+    <t>Spring roll (1)</t>
+  </si>
+  <si>
+    <t>Chicken egg roll (1)</t>
+  </si>
+  <si>
+    <t>Chicken dumplings (6)</t>
+  </si>
+  <si>
+    <t>Shrimp Tempura (3)</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -376,12 +414,99 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D852D101-3741-4B56-A42E-178EC62FB9FE}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>6.99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>7.49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>8.2899999999999991</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>7.19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>8.19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>1.29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>2.4900000000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>2.99</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>